<commit_message>
Chris checked his analyses and adjusted some parts for final data analysis
</commit_message>
<xml_diff>
--- a/tilburg data.xlsx
+++ b/tilburg data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\reproducibility project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chjh\Dropbox\projects\2014rpp\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -9240,8 +9240,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -9299,6 +9297,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9630,10 +9630,10 @@
   <dimension ref="A1:EC170"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="DJ2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="DN9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="EA2" sqref="EA2"/>
+      <selection pane="bottomRight" activeCell="EC1" sqref="EC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9679,16 +9679,23 @@
     <col min="69" max="69" width="19.42578125" customWidth="1"/>
     <col min="70" max="77" width="12.7109375" customWidth="1"/>
     <col min="78" max="78" width="15.5703125" customWidth="1"/>
-    <col min="79" max="114" width="12.7109375" customWidth="1"/>
-    <col min="115" max="115" width="0.85546875" style="146" customWidth="1"/>
-    <col min="116" max="118" width="12.7109375" hidden="1" customWidth="1"/>
-    <col min="119" max="119" width="1.28515625" hidden="1" customWidth="1"/>
-    <col min="120" max="120" width="17.85546875" hidden="1" customWidth="1"/>
-    <col min="121" max="121" width="9.7109375" hidden="1" customWidth="1"/>
-    <col min="122" max="125" width="12.7109375" hidden="1" customWidth="1"/>
-    <col min="126" max="126" width="12.7109375" customWidth="1"/>
-    <col min="127" max="130" width="8.7109375" customWidth="1"/>
-    <col min="131" max="132" width="8.7109375" style="165" customWidth="1"/>
+    <col min="79" max="113" width="12.7109375" customWidth="1"/>
+    <col min="114" max="114" width="7.140625" customWidth="1"/>
+    <col min="115" max="115" width="7.5703125" style="146" customWidth="1"/>
+    <col min="116" max="116" width="18.28515625" customWidth="1"/>
+    <col min="117" max="117" width="22.140625" customWidth="1"/>
+    <col min="118" max="119" width="9" customWidth="1"/>
+    <col min="120" max="120" width="15.85546875" customWidth="1"/>
+    <col min="121" max="121" width="19.140625" customWidth="1"/>
+    <col min="122" max="122" width="10.140625" customWidth="1"/>
+    <col min="123" max="123" width="16.5703125" customWidth="1"/>
+    <col min="124" max="124" width="15.140625" customWidth="1"/>
+    <col min="125" max="125" width="10" customWidth="1"/>
+    <col min="126" max="126" width="7" customWidth="1"/>
+    <col min="127" max="127" width="26.5703125" customWidth="1"/>
+    <col min="128" max="128" width="19.42578125" customWidth="1"/>
+    <col min="129" max="130" width="8.7109375" customWidth="1"/>
+    <col min="131" max="132" width="8.7109375" style="163" customWidth="1"/>
     <col min="133" max="133" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10080,13 +10087,13 @@
       <c r="DY1" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="EA1" s="164" t="s">
+      <c r="EA1" s="162" t="s">
         <v>2863</v>
       </c>
-      <c r="EB1" s="164" t="s">
+      <c r="EB1" s="162" t="s">
         <v>2864</v>
       </c>
-      <c r="EC1" s="164" t="s">
+      <c r="EC1" s="162" t="s">
         <v>2865</v>
       </c>
     </row>
@@ -10458,11 +10465,11 @@
       <c r="DY2" s="29" t="s">
         <v>292</v>
       </c>
-      <c r="EA2" s="165">
+      <c r="EA2" s="163">
         <f>IF(DH2 &lt; 0.05,1,0)</f>
         <v>1</v>
       </c>
-      <c r="EB2" s="165">
+      <c r="EB2" s="163">
         <f>IF(DT2 &lt; 0.05,1,0)</f>
         <v>0</v>
       </c>
@@ -10845,11 +10852,11 @@
       <c r="DY3" s="29" t="s">
         <v>341</v>
       </c>
-      <c r="EA3" s="165">
+      <c r="EA3" s="163">
         <f t="shared" ref="EA3:EA66" si="0">IF(DH3 &lt; 0.05,1,0)</f>
         <v>1</v>
       </c>
-      <c r="EB3" s="165">
+      <c r="EB3" s="163">
         <f t="shared" ref="EA3:EB66" si="1">IF(DT3 &lt; 0.05,1,0)</f>
         <v>0</v>
       </c>
@@ -11222,7 +11229,7 @@
         <v>0.22898882700000001</v>
       </c>
       <c r="DU4" s="90"/>
-      <c r="DV4" s="153">
+      <c r="DV4" s="151">
         <f>-0.215243835</f>
         <v>-0.21524383499999999</v>
       </c>
@@ -11233,11 +11240,11 @@
       <c r="DY4" s="29" t="s">
         <v>368</v>
       </c>
-      <c r="EA4" s="165">
+      <c r="EA4" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB4" s="165">
+      <c r="EB4" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -11604,7 +11611,7 @@
         <v>0.92041908900000002</v>
       </c>
       <c r="DU5" s="90"/>
-      <c r="DV5" s="153">
+      <c r="DV5" s="151">
         <f>-0.006108358</f>
         <v>-6.1083580000000004E-3</v>
       </c>
@@ -11615,11 +11622,11 @@
       <c r="DY5" s="29" t="s">
         <v>397</v>
       </c>
-      <c r="EA5" s="165">
+      <c r="EA5" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB5" s="165">
+      <c r="EB5" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -11998,11 +12005,11 @@
       <c r="DY6" s="29" t="s">
         <v>436</v>
       </c>
-      <c r="EA6" s="165">
+      <c r="EA6" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB6" s="165">
+      <c r="EB6" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -12383,11 +12390,11 @@
       <c r="DY7" s="29" t="s">
         <v>465</v>
       </c>
-      <c r="EA7" s="165">
+      <c r="EA7" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB7" s="165">
+      <c r="EB7" s="163">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -12770,11 +12777,11 @@
       <c r="DY8" s="29" t="s">
         <v>491</v>
       </c>
-      <c r="EA8" s="165">
+      <c r="EA8" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB8" s="165">
+      <c r="EB8" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -13143,7 +13150,7 @@
         <v>0.539998592</v>
       </c>
       <c r="DU9" s="90"/>
-      <c r="DV9" s="153">
+      <c r="DV9" s="151">
         <f>-0.110614348</f>
         <v>-0.110614348</v>
       </c>
@@ -13154,11 +13161,11 @@
       <c r="DY9" s="15" t="s">
         <v>513</v>
       </c>
-      <c r="EA9" s="165">
+      <c r="EA9" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB9" s="165">
+      <c r="EB9" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -13829,11 +13836,11 @@
       <c r="DY11" s="29" t="s">
         <v>551</v>
       </c>
-      <c r="EA11" s="165">
+      <c r="EA11" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB11" s="165">
+      <c r="EB11" s="163">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -14210,11 +14217,11 @@
       <c r="DY12" s="29" t="s">
         <v>574</v>
       </c>
-      <c r="EA12" s="165">
+      <c r="EA12" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB12" s="165">
+      <c r="EB12" s="163">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -14591,11 +14598,11 @@
       <c r="DY13" s="29" t="s">
         <v>596</v>
       </c>
-      <c r="EA13" s="165">
+      <c r="EA13" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB13" s="165">
+      <c r="EB13" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -14972,11 +14979,11 @@
       <c r="DY14" s="29" t="s">
         <v>619</v>
       </c>
-      <c r="EA14" s="165">
+      <c r="EA14" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB14" s="165">
+      <c r="EB14" s="163">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -15569,13 +15576,13 @@
       <c r="DE16" s="41" t="s">
         <v>287</v>
       </c>
-      <c r="DF16" s="158">
+      <c r="DF16" s="156">
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="DG16" s="20">
         <v>5.6747408999999999E-2</v>
       </c>
-      <c r="DH16" s="157">
+      <c r="DH16" s="155">
         <f>0.056747409/2</f>
         <v>2.8373704499999999E-2</v>
       </c>
@@ -15604,13 +15611,13 @@
       <c r="DQ16" s="125" t="s">
         <v>287</v>
       </c>
-      <c r="DR16" s="154">
+      <c r="DR16" s="152">
         <v>1E-4</v>
       </c>
-      <c r="DS16" s="156">
+      <c r="DS16" s="154">
         <v>1.01E-4</v>
       </c>
-      <c r="DT16" s="155">
+      <c r="DT16" s="153">
         <f>0.000101/2</f>
         <v>5.0500000000000001E-5</v>
       </c>
@@ -15625,11 +15632,11 @@
       <c r="DY16" s="29" t="s">
         <v>491</v>
       </c>
-      <c r="EA16" s="165">
+      <c r="EA16" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB16" s="165">
+      <c r="EB16" s="163">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -16199,11 +16206,11 @@
       <c r="DY18" s="29" t="s">
         <v>682</v>
       </c>
-      <c r="EA18" s="165">
+      <c r="EA18" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB18" s="165">
+      <c r="EB18" s="163">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -16764,11 +16771,11 @@
       <c r="DY20" s="29" t="s">
         <v>711</v>
       </c>
-      <c r="EA20" s="165">
+      <c r="EA20" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB20" s="165">
+      <c r="EB20" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -17147,11 +17154,11 @@
       <c r="DY21" s="29" t="s">
         <v>397</v>
       </c>
-      <c r="EA21" s="165">
+      <c r="EA21" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB21" s="165">
+      <c r="EB21" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -17709,11 +17716,11 @@
       <c r="DY23" s="29" t="s">
         <v>760</v>
       </c>
-      <c r="EA23" s="165">
+      <c r="EA23" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB23" s="165">
+      <c r="EB23" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -18243,11 +18250,11 @@
       <c r="DY25" s="29" t="s">
         <v>780</v>
       </c>
-      <c r="EA25" s="165">
+      <c r="EA25" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB25" s="165">
+      <c r="EB25" s="163">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -18618,11 +18625,11 @@
         <v>291</v>
       </c>
       <c r="DY26" s="86"/>
-      <c r="EA26" s="165">
+      <c r="EA26" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB26" s="165">
+      <c r="EB26" s="163">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -19002,11 +19009,11 @@
       <c r="DY27" s="29" t="s">
         <v>397</v>
       </c>
-      <c r="EA27" s="165">
+      <c r="EA27" s="163">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="EB27" s="165">
+      <c r="EB27" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -19383,11 +19390,11 @@
       <c r="DY28" s="29" t="s">
         <v>843</v>
       </c>
-      <c r="EA28" s="165">
+      <c r="EA28" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB28" s="165">
+      <c r="EB28" s="163">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -19768,10 +19775,10 @@
       <c r="DY29" s="29" t="s">
         <v>574</v>
       </c>
-      <c r="EA29" s="167">
-        <v>1</v>
-      </c>
-      <c r="EB29" s="165">
+      <c r="EA29" s="165">
+        <v>1</v>
+      </c>
+      <c r="EB29" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -20150,11 +20157,11 @@
       <c r="DY30" s="29" t="s">
         <v>797</v>
       </c>
-      <c r="EA30" s="165">
+      <c r="EA30" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB30" s="165">
+      <c r="EB30" s="163">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -20954,11 +20961,11 @@
       <c r="DY33" s="29" t="s">
         <v>927</v>
       </c>
-      <c r="EA33" s="165">
+      <c r="EA33" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB33" s="165">
+      <c r="EB33" s="163">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -21339,11 +21346,11 @@
       <c r="DY34" s="29" t="s">
         <v>491</v>
       </c>
-      <c r="EA34" s="165">
+      <c r="EA34" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB34" s="165">
+      <c r="EB34" s="163">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -21753,10 +21760,10 @@
       <c r="CL36" s="39">
         <v>4723</v>
       </c>
-      <c r="CM36" s="151" t="s">
+      <c r="CM36" s="172" t="s">
         <v>549</v>
       </c>
-      <c r="CN36" s="152"/>
+      <c r="CN36" s="173"/>
       <c r="CO36" s="67"/>
       <c r="CP36" s="67"/>
       <c r="CQ36" s="67"/>
@@ -22194,11 +22201,11 @@
       <c r="DY37" s="29" t="s">
         <v>397</v>
       </c>
-      <c r="EA37" s="165">
+      <c r="EA37" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB37" s="165">
+      <c r="EB37" s="163">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -22575,10 +22582,10 @@
       <c r="DY38" s="29" t="s">
         <v>710</v>
       </c>
-      <c r="EA38" s="167">
-        <v>1</v>
-      </c>
-      <c r="EB38" s="165">
+      <c r="EA38" s="165">
+        <v>1</v>
+      </c>
+      <c r="EB38" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -23119,11 +23126,11 @@
       <c r="DY40" s="29" t="s">
         <v>1035</v>
       </c>
-      <c r="EA40" s="165">
+      <c r="EA40" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB40" s="165">
+      <c r="EB40" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -24144,11 +24151,11 @@
       <c r="DY44" s="29" t="s">
         <v>291</v>
       </c>
-      <c r="EA44" s="165">
+      <c r="EA44" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB44" s="165">
+      <c r="EB44" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -24529,11 +24536,11 @@
       <c r="DY45" s="29" t="s">
         <v>1104</v>
       </c>
-      <c r="EA45" s="165">
+      <c r="EA45" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB45" s="165">
+      <c r="EB45" s="163">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -25044,7 +25051,7 @@
       <c r="DG47" s="20">
         <v>0</v>
       </c>
-      <c r="DH47" s="157">
+      <c r="DH47" s="155">
         <v>0</v>
       </c>
       <c r="DI47" s="20"/>
@@ -25078,7 +25085,7 @@
       <c r="DS47" s="90">
         <v>0</v>
       </c>
-      <c r="DT47" s="157">
+      <c r="DT47" s="155">
         <v>0</v>
       </c>
       <c r="DU47" s="90"/>
@@ -25092,11 +25099,11 @@
       <c r="DY47" s="29" t="s">
         <v>1143</v>
       </c>
-      <c r="EA47" s="165">
+      <c r="EA47" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB47" s="165">
+      <c r="EB47" s="163">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -25690,13 +25697,13 @@
       <c r="DO49" s="95">
         <v>192</v>
       </c>
-      <c r="DP49" s="154">
+      <c r="DP49" s="152">
         <v>-0.72554799999999997</v>
       </c>
       <c r="DQ49" s="125" t="s">
         <v>287</v>
       </c>
-      <c r="DR49" s="154">
+      <c r="DR49" s="152">
         <v>0.47</v>
       </c>
       <c r="DS49" s="90">
@@ -25716,11 +25723,11 @@
       <c r="DY49" s="29" t="s">
         <v>1176</v>
       </c>
-      <c r="EA49" s="165">
+      <c r="EA49" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB49" s="165">
+      <c r="EB49" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -26091,7 +26098,7 @@
         <v>0.77797708200000004</v>
       </c>
       <c r="DU50" s="96"/>
-      <c r="DV50" s="168">
+      <c r="DV50" s="166">
         <f>-0.030485538</f>
         <v>-3.0485538E-2</v>
       </c>
@@ -26102,11 +26109,11 @@
       <c r="DY50" s="29" t="s">
         <v>291</v>
       </c>
-      <c r="EA50" s="165">
+      <c r="EA50" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB50" s="165">
+      <c r="EB50" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -26483,11 +26490,11 @@
       <c r="DY51" s="29" t="s">
         <v>1212</v>
       </c>
-      <c r="EA51" s="165">
+      <c r="EA51" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB51" s="165">
+      <c r="EB51" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -27180,11 +27187,11 @@
       <c r="DY53" s="29" t="s">
         <v>1250</v>
       </c>
-      <c r="EA53" s="165">
+      <c r="EA53" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB53" s="165">
+      <c r="EB53" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -27561,11 +27568,11 @@
       <c r="DY54" s="29" t="s">
         <v>822</v>
       </c>
-      <c r="EA54" s="165">
+      <c r="EA54" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB54" s="165">
+      <c r="EB54" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -28127,11 +28134,11 @@
       <c r="DY56" s="29" t="s">
         <v>291</v>
       </c>
-      <c r="EA56" s="165">
+      <c r="EA56" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB56" s="165">
+      <c r="EB56" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -28500,7 +28507,7 @@
         <v>0.79626739400000002</v>
       </c>
       <c r="DU57" s="90"/>
-      <c r="DV57" s="153">
+      <c r="DV57" s="151">
         <f>-0.042140104</f>
         <v>-4.2140103999999998E-2</v>
       </c>
@@ -28511,11 +28518,11 @@
       <c r="DY57" s="29" t="s">
         <v>797</v>
       </c>
-      <c r="EA57" s="165">
+      <c r="EA57" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB57" s="165">
+      <c r="EB57" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -29158,11 +29165,11 @@
       <c r="DY59" s="29" t="s">
         <v>435</v>
       </c>
-      <c r="EA59" s="165">
+      <c r="EA59" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB59" s="165">
+      <c r="EB59" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -29491,7 +29498,7 @@
       <c r="DG60" s="20" t="s">
         <v>512</v>
       </c>
-      <c r="DH60" s="160"/>
+      <c r="DH60" s="158"/>
       <c r="DI60" s="20"/>
       <c r="DJ60" s="20" t="s">
         <v>512</v>
@@ -29517,9 +29524,9 @@
         <v>1E-3</v>
       </c>
       <c r="DS60" s="90"/>
-      <c r="DT60" s="160"/>
+      <c r="DT60" s="158"/>
       <c r="DU60" s="90"/>
-      <c r="DV60" s="159"/>
+      <c r="DV60" s="157"/>
       <c r="DW60" s="148"/>
       <c r="DX60" s="29" t="s">
         <v>1354</v>
@@ -29527,15 +29534,15 @@
       <c r="DY60" s="29" t="s">
         <v>1354</v>
       </c>
-      <c r="EA60" s="166">
+      <c r="EA60" s="164">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="EB60" s="166">
+      <c r="EB60" s="164">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="EC60" s="172">
+      <c r="EC60" s="170">
         <v>0</v>
       </c>
     </row>
@@ -30080,7 +30087,7 @@
         <v>0.94425724600000005</v>
       </c>
       <c r="DU62" s="96"/>
-      <c r="DV62" s="168">
+      <c r="DV62" s="166">
         <f>-0.004719346</f>
         <v>-4.7193460000000001E-3</v>
       </c>
@@ -30091,11 +30098,11 @@
       <c r="DY62" s="29" t="s">
         <v>1384</v>
       </c>
-      <c r="EA62" s="165">
+      <c r="EA62" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB62" s="165">
+      <c r="EB62" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -30655,11 +30662,11 @@
       <c r="DY64" s="29" t="s">
         <v>1411</v>
       </c>
-      <c r="EA64" s="165">
+      <c r="EA64" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB64" s="165">
+      <c r="EB64" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -31038,11 +31045,11 @@
       <c r="DY65" s="29" t="s">
         <v>291</v>
       </c>
-      <c r="EA65" s="165">
+      <c r="EA65" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB65" s="165">
+      <c r="EB65" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -31421,11 +31428,11 @@
       <c r="DY66" s="29" t="s">
         <v>1457</v>
       </c>
-      <c r="EA66" s="165">
+      <c r="EA66" s="163">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="EB66" s="165">
+      <c r="EB66" s="163">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -32142,16 +32149,16 @@
       <c r="DY69" s="29" t="s">
         <v>291</v>
       </c>
-      <c r="EA69" s="165">
-        <f t="shared" ref="EA67:EA130" si="3">IF(DH69 &lt; 0.05,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="EB69" s="165">
-        <f t="shared" ref="EB67:EB130" si="4">IF(DT69 &lt; 0.05,1,0)</f>
+      <c r="EA69" s="163">
+        <f t="shared" ref="EA69:EA128" si="3">IF(DH69 &lt; 0.05,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="EB69" s="163">
+        <f t="shared" ref="EB69:EB130" si="4">IF(DT69 &lt; 0.05,1,0)</f>
         <v>0</v>
       </c>
       <c r="EC69" s="147">
-        <f t="shared" ref="EC67:EC130" si="5">IF(DJ69&gt;DV69,1,0)</f>
+        <f t="shared" ref="EC69:EC130" si="5">IF(DJ69&gt;DV69,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -32326,7 +32333,7 @@
       <c r="BF70" s="29" t="s">
         <v>1497</v>
       </c>
-      <c r="BG70" s="171">
+      <c r="BG70" s="169">
         <v>0.78</v>
       </c>
       <c r="BH70" s="33"/>
@@ -32381,7 +32388,7 @@
       <c r="BY70" s="30">
         <v>0.99</v>
       </c>
-      <c r="BZ70" s="171">
+      <c r="BZ70" s="169">
         <v>0.77</v>
       </c>
       <c r="CA70" s="29" t="s">
@@ -32505,7 +32512,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="DU70" s="90"/>
-      <c r="DV70" s="159"/>
+      <c r="DV70" s="157"/>
       <c r="DW70" s="148"/>
       <c r="DX70" s="29" t="s">
         <v>1496</v>
@@ -32513,15 +32520,15 @@
       <c r="DY70" s="29" t="s">
         <v>1496</v>
       </c>
-      <c r="EA70" s="165">
+      <c r="EA70" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB70" s="165">
+      <c r="EB70" s="163">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="EC70" s="172">
+      <c r="EC70" s="170">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -33081,11 +33088,11 @@
       <c r="DY72" s="29" t="s">
         <v>797</v>
       </c>
-      <c r="EA72" s="165">
+      <c r="EA72" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB72" s="165">
+      <c r="EB72" s="163">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -33466,11 +33473,11 @@
       <c r="DY73" s="29" t="s">
         <v>1457</v>
       </c>
-      <c r="EA73" s="165">
+      <c r="EA73" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB73" s="165">
+      <c r="EB73" s="163">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -33847,11 +33854,11 @@
       <c r="DY74" s="29" t="s">
         <v>1564</v>
       </c>
-      <c r="EA74" s="165">
+      <c r="EA74" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB74" s="165">
+      <c r="EB74" s="163">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -34733,7 +34740,7 @@
         <v>0.75800000000000001</v>
       </c>
       <c r="DU78" s="90"/>
-      <c r="DV78" s="159"/>
+      <c r="DV78" s="157"/>
       <c r="DW78" s="148"/>
       <c r="DX78" s="15" t="s">
         <v>291</v>
@@ -34741,15 +34748,15 @@
       <c r="DY78" s="15" t="s">
         <v>1608</v>
       </c>
-      <c r="EA78" s="165">
+      <c r="EA78" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB78" s="165">
+      <c r="EB78" s="163">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="EC78" s="173"/>
+      <c r="EC78" s="171"/>
     </row>
     <row r="79" spans="1:133" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="14">
@@ -35599,11 +35606,11 @@
       <c r="DY81" s="29" t="s">
         <v>1651</v>
       </c>
-      <c r="EA81" s="165">
+      <c r="EA81" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB81" s="165">
+      <c r="EB81" s="163">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -35972,7 +35979,7 @@
         <v>0.23383009900000001</v>
       </c>
       <c r="DU82" s="90"/>
-      <c r="DV82" s="153">
+      <c r="DV82" s="151">
         <f>-0.101637251</f>
         <v>-0.101637251</v>
       </c>
@@ -35983,11 +35990,11 @@
       <c r="DY82" s="29" t="s">
         <v>1670</v>
       </c>
-      <c r="EA82" s="165">
+      <c r="EA82" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB82" s="165">
+      <c r="EB82" s="163">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -36366,11 +36373,11 @@
       <c r="DY83" s="29" t="s">
         <v>1689</v>
       </c>
-      <c r="EA83" s="165">
+      <c r="EA83" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB83" s="165">
+      <c r="EB83" s="163">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -36894,11 +36901,11 @@
       <c r="DY85" s="29" t="s">
         <v>1711</v>
       </c>
-      <c r="EA85" s="165">
+      <c r="EA85" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB85" s="165">
+      <c r="EB85" s="163">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -37459,11 +37466,11 @@
       <c r="DY87" s="29" t="s">
         <v>1727</v>
       </c>
-      <c r="EA87" s="165">
+      <c r="EA87" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB87" s="165">
+      <c r="EB87" s="163">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -37840,11 +37847,11 @@
       <c r="DY88" s="29" t="s">
         <v>1457</v>
       </c>
-      <c r="EA88" s="165">
+      <c r="EA88" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB88" s="165">
+      <c r="EB88" s="163">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -38423,11 +38430,11 @@
       <c r="DY90" s="29" t="s">
         <v>1764</v>
       </c>
-      <c r="EA90" s="165">
+      <c r="EA90" s="163">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="EB90" s="165">
+      <c r="EB90" s="163">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -39350,17 +39357,17 @@
       <c r="DQ94" s="125" t="s">
         <v>287</v>
       </c>
-      <c r="DR94" s="161">
+      <c r="DR94" s="159">
         <v>0.26500000000000001</v>
       </c>
-      <c r="DS94" s="162">
+      <c r="DS94" s="160">
         <v>0.26496530000000001</v>
       </c>
-      <c r="DT94" s="162">
+      <c r="DT94" s="160">
         <v>0.26496530000000001</v>
       </c>
       <c r="DU94" s="90"/>
-      <c r="DV94" s="163">
+      <c r="DV94" s="161">
         <v>-0.1351</v>
       </c>
       <c r="DW94" s="148"/>
@@ -39370,11 +39377,11 @@
       <c r="DY94" s="29" t="s">
         <v>1811</v>
       </c>
-      <c r="EA94" s="165">
+      <c r="EA94" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB94" s="165">
+      <c r="EB94" s="163">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -39755,11 +39762,11 @@
       <c r="DY95" s="29" t="s">
         <v>1832</v>
       </c>
-      <c r="EA95" s="165">
+      <c r="EA95" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB95" s="165">
+      <c r="EB95" s="163">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -40620,7 +40627,7 @@
         <v>0.15443058600000001</v>
       </c>
       <c r="DU98" s="90"/>
-      <c r="DV98" s="153">
+      <c r="DV98" s="151">
         <f>-0.036935346</f>
         <v>-3.6935346000000001E-2</v>
       </c>
@@ -40631,11 +40638,11 @@
       <c r="DY98" s="29" t="s">
         <v>1872</v>
       </c>
-      <c r="EA98" s="165">
+      <c r="EA98" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB98" s="165">
+      <c r="EB98" s="163">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -42112,10 +42119,10 @@
       <c r="DY105" s="29" t="s">
         <v>1711</v>
       </c>
-      <c r="EA105" s="167">
-        <v>1</v>
-      </c>
-      <c r="EB105" s="165">
+      <c r="EA105" s="165">
+        <v>1</v>
+      </c>
+      <c r="EB105" s="163">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -42768,7 +42775,7 @@
         <v>0.13203104399999999</v>
       </c>
       <c r="DU107" s="90"/>
-      <c r="DV107" s="153">
+      <c r="DV107" s="151">
         <f>-0.222920955</f>
         <v>-0.222920955</v>
       </c>
@@ -42779,11 +42786,11 @@
       <c r="DY107" s="29" t="s">
         <v>1970</v>
       </c>
-      <c r="EA107" s="165">
+      <c r="EA107" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB107" s="165">
+      <c r="EB107" s="163">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -43166,11 +43173,11 @@
       <c r="DY108" s="29" t="s">
         <v>1995</v>
       </c>
-      <c r="EA108" s="165">
+      <c r="EA108" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB108" s="165">
+      <c r="EB108" s="163">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -43945,11 +43952,11 @@
       <c r="DY111" s="29" t="s">
         <v>292</v>
       </c>
-      <c r="EA111" s="165">
+      <c r="EA111" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB111" s="165">
+      <c r="EB111" s="163">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -44328,11 +44335,11 @@
       <c r="DY112" s="29" t="s">
         <v>1457</v>
       </c>
-      <c r="EA112" s="165">
+      <c r="EA112" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB112" s="165">
+      <c r="EB112" s="163">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -44709,11 +44716,11 @@
       <c r="DY113" s="29" t="s">
         <v>291</v>
       </c>
-      <c r="EA113" s="165">
+      <c r="EA113" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB113" s="165">
+      <c r="EB113" s="163">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -45092,11 +45099,11 @@
       <c r="DY114" s="29" t="s">
         <v>2098</v>
       </c>
-      <c r="EA114" s="165">
+      <c r="EA114" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB114" s="165">
+      <c r="EB114" s="163">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -45475,11 +45482,11 @@
       <c r="DY115" s="29" t="s">
         <v>710</v>
       </c>
-      <c r="EA115" s="165">
+      <c r="EA115" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB115" s="165">
+      <c r="EB115" s="163">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -45848,7 +45855,7 @@
         <v>0.19170092399999999</v>
       </c>
       <c r="DU116" s="90"/>
-      <c r="DV116" s="153">
+      <c r="DV116" s="151">
         <f>-0.450187899</f>
         <v>-0.450187899</v>
       </c>
@@ -45859,11 +45866,11 @@
       <c r="DY116" s="29" t="s">
         <v>1172</v>
       </c>
-      <c r="EA116" s="165">
+      <c r="EA116" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB116" s="165">
+      <c r="EB116" s="163">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -46244,11 +46251,11 @@
       <c r="DY117" s="29" t="s">
         <v>2153</v>
       </c>
-      <c r="EA117" s="165">
+      <c r="EA117" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB117" s="165">
+      <c r="EB117" s="163">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -46627,11 +46634,11 @@
       <c r="DY118" s="29" t="s">
         <v>291</v>
       </c>
-      <c r="EA118" s="165">
+      <c r="EA118" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB118" s="165">
+      <c r="EB118" s="163">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -46996,7 +47003,7 @@
         <v>0.539024693</v>
       </c>
       <c r="DU119" s="90"/>
-      <c r="DV119" s="153">
+      <c r="DV119" s="151">
         <f>-0.048918238</f>
         <v>-4.8918238000000003E-2</v>
       </c>
@@ -47007,11 +47014,11 @@
       <c r="DY119" s="29" t="s">
         <v>2189</v>
       </c>
-      <c r="EA119" s="165">
+      <c r="EA119" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB119" s="165">
+      <c r="EB119" s="163">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -47521,7 +47528,7 @@
       <c r="DG121" s="20">
         <v>3.4266919E-2</v>
       </c>
-      <c r="DH121" s="157">
+      <c r="DH121" s="155">
         <f>0.034266919/2</f>
         <v>1.71334595E-2</v>
       </c>
@@ -47552,7 +47559,7 @@
       <c r="DS121" s="90">
         <v>0.106230061</v>
       </c>
-      <c r="DT121" s="157">
+      <c r="DT121" s="155">
         <f>0.106230061/2</f>
         <v>5.31150305E-2</v>
       </c>
@@ -47567,11 +47574,11 @@
       <c r="DY121" s="29" t="s">
         <v>2217</v>
       </c>
-      <c r="EA121" s="165">
+      <c r="EA121" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB121" s="165">
+      <c r="EB121" s="163">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -47946,11 +47953,11 @@
       <c r="DY122" s="29" t="s">
         <v>2232</v>
       </c>
-      <c r="EA122" s="165">
+      <c r="EA122" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB122" s="165">
+      <c r="EB122" s="163">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -48333,11 +48340,11 @@
       <c r="DY123" s="29" t="s">
         <v>491</v>
       </c>
-      <c r="EA123" s="165">
+      <c r="EA123" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB123" s="165">
+      <c r="EB123" s="163">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -48752,7 +48759,7 @@
       <c r="BS125" s="30">
         <v>0.79</v>
       </c>
-      <c r="BT125" s="170" t="s">
+      <c r="BT125" s="168" t="s">
         <v>375</v>
       </c>
       <c r="BU125" s="31"/>
@@ -48906,7 +48913,7 @@
         <v>0.77815663199999996</v>
       </c>
       <c r="DU125" s="90"/>
-      <c r="DV125" s="153">
+      <c r="DV125" s="151">
         <f>-0.034279559</f>
         <v>-3.4279559000000001E-2</v>
       </c>
@@ -48917,11 +48924,11 @@
       <c r="DY125" s="29" t="s">
         <v>291</v>
       </c>
-      <c r="EA125" s="165">
+      <c r="EA125" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB125" s="165">
+      <c r="EB125" s="163">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -49659,11 +49666,11 @@
       <c r="DY128" s="29" t="s">
         <v>491</v>
       </c>
-      <c r="EA128" s="165">
+      <c r="EA128" s="163">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EB128" s="165">
+      <c r="EB128" s="163">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -49914,10 +49921,10 @@
       <c r="CO129" s="37" t="s">
         <v>328</v>
       </c>
-      <c r="CP129" s="151" t="s">
+      <c r="CP129" s="172" t="s">
         <v>2317</v>
       </c>
-      <c r="CQ129" s="152"/>
+      <c r="CQ129" s="173"/>
       <c r="CR129" s="67"/>
       <c r="CS129" s="37" t="s">
         <v>332</v>
@@ -50352,10 +50359,10 @@
       <c r="DY130" s="29" t="s">
         <v>2334</v>
       </c>
-      <c r="EA130" s="167">
-        <v>1</v>
-      </c>
-      <c r="EB130" s="165">
+      <c r="EA130" s="165">
+        <v>1</v>
+      </c>
+      <c r="EB130" s="163">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -51029,16 +51036,16 @@
       <c r="DY133" s="29" t="s">
         <v>2362</v>
       </c>
-      <c r="EA133" s="165">
-        <f t="shared" ref="EA131:EA168" si="6">IF(DH133 &lt; 0.05,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="EB133" s="165">
-        <f t="shared" ref="EB131:EB168" si="7">IF(DT133 &lt; 0.05,1,0)</f>
+      <c r="EA133" s="163">
+        <f t="shared" ref="EA133:EA168" si="6">IF(DH133 &lt; 0.05,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="EB133" s="163">
+        <f t="shared" ref="EB133:EB168" si="7">IF(DT133 &lt; 0.05,1,0)</f>
         <v>0</v>
       </c>
       <c r="EC133" s="147">
-        <f t="shared" ref="EC131:EC168" si="8">IF(DJ133&gt;DV133,1,0)</f>
+        <f t="shared" ref="EC133:EC168" si="8">IF(DJ133&gt;DV133,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -51410,11 +51417,11 @@
       <c r="DY134" s="29" t="s">
         <v>291</v>
       </c>
-      <c r="EA134" s="165">
+      <c r="EA134" s="163">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="EB134" s="165">
+      <c r="EB134" s="163">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
@@ -51741,7 +51748,7 @@
       <c r="DE135" s="133" t="s">
         <v>1994</v>
       </c>
-      <c r="DF135" s="154">
+      <c r="DF135" s="152">
         <v>2.3E-2</v>
       </c>
       <c r="DG135" s="148" t="s">
@@ -51769,19 +51776,19 @@
       <c r="DO135" s="149">
         <v>234</v>
       </c>
-      <c r="DP135" s="154">
+      <c r="DP135" s="152">
         <v>8.8360000000000003</v>
       </c>
       <c r="DQ135" s="149" t="s">
         <v>287</v>
       </c>
-      <c r="DR135" s="154">
+      <c r="DR135" s="152">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="DS135" s="156">
+      <c r="DS135" s="154">
         <v>2.4100000000000002E-16</v>
       </c>
-      <c r="DT135" s="156">
+      <c r="DT135" s="154">
         <v>2.4100000000000002E-16</v>
       </c>
       <c r="DU135" s="90"/>
@@ -51795,11 +51802,11 @@
       <c r="DY135" s="29" t="s">
         <v>2395</v>
       </c>
-      <c r="EA135" s="165">
+      <c r="EA135" s="163">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="EB135" s="165">
+      <c r="EB135" s="163">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
@@ -52180,11 +52187,11 @@
       <c r="DY136" s="29" t="s">
         <v>2415</v>
       </c>
-      <c r="EA136" s="165">
+      <c r="EA136" s="163">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="EB136" s="165">
+      <c r="EB136" s="163">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
@@ -52463,10 +52470,10 @@
       <c r="CO137" s="37" t="s">
         <v>330</v>
       </c>
-      <c r="CP137" s="151" t="s">
+      <c r="CP137" s="172" t="s">
         <v>2435</v>
       </c>
-      <c r="CQ137" s="152"/>
+      <c r="CQ137" s="173"/>
       <c r="CR137" s="37" t="s">
         <v>382</v>
       </c>
@@ -52563,11 +52570,11 @@
       <c r="DY137" s="29" t="s">
         <v>797</v>
       </c>
-      <c r="EA137" s="165">
+      <c r="EA137" s="163">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="EB137" s="165">
+      <c r="EB137" s="163">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -53252,7 +53259,7 @@
       <c r="DG140" s="20">
         <v>5.4252270000000003E-3</v>
       </c>
-      <c r="DH140" s="157">
+      <c r="DH140" s="155">
         <f>0.005425227/2</f>
         <v>2.7126135000000002E-3</v>
       </c>
@@ -53287,7 +53294,7 @@
       <c r="DS140" s="90">
         <v>4.3546399999999999E-4</v>
       </c>
-      <c r="DT140" s="157">
+      <c r="DT140" s="155">
         <f>0.000435464/2</f>
         <v>2.1773199999999999E-4</v>
       </c>
@@ -53302,11 +53309,11 @@
       <c r="DY140" s="29" t="s">
         <v>2472</v>
       </c>
-      <c r="EA140" s="165">
+      <c r="EA140" s="163">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="EB140" s="165">
+      <c r="EB140" s="163">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
@@ -53685,11 +53692,11 @@
       <c r="DY141" s="29" t="s">
         <v>291</v>
       </c>
-      <c r="EA141" s="165">
+      <c r="EA141" s="163">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="EB141" s="165">
+      <c r="EB141" s="163">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -54344,11 +54351,11 @@
       <c r="DY143" s="29" t="s">
         <v>292</v>
       </c>
-      <c r="EA143" s="165">
+      <c r="EA143" s="163">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="EB143" s="165">
+      <c r="EB143" s="163">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
@@ -54727,11 +54734,11 @@
       <c r="DY144" s="29" t="s">
         <v>2543</v>
       </c>
-      <c r="EA144" s="165">
+      <c r="EA144" s="163">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="EB144" s="165">
+      <c r="EB144" s="163">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -55261,11 +55268,11 @@
       <c r="DY146" s="29" t="s">
         <v>2563</v>
       </c>
-      <c r="EA146" s="165">
+      <c r="EA146" s="163">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="EB146" s="165">
+      <c r="EB146" s="163">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
@@ -55650,11 +55657,11 @@
       <c r="DY147" s="29" t="s">
         <v>491</v>
       </c>
-      <c r="EA147" s="165">
+      <c r="EA147" s="163">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="EB147" s="165">
+      <c r="EB147" s="163">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -56287,7 +56294,7 @@
         <v>0.62752089600000005</v>
       </c>
       <c r="DU149" s="90"/>
-      <c r="DV149" s="153">
+      <c r="DV149" s="151">
         <f>-0.030172295</f>
         <v>-3.0172294999999998E-2</v>
       </c>
@@ -56298,11 +56305,11 @@
       <c r="DY149" s="29" t="s">
         <v>2611</v>
       </c>
-      <c r="EA149" s="165">
+      <c r="EA149" s="163">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="EB149" s="165">
+      <c r="EB149" s="163">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -56679,11 +56686,11 @@
       <c r="DY150" s="29" t="s">
         <v>2615</v>
       </c>
-      <c r="EA150" s="165">
+      <c r="EA150" s="163">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="EB150" s="165">
+      <c r="EB150" s="163">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -57060,11 +57067,11 @@
       <c r="DY151" s="29" t="s">
         <v>2635</v>
       </c>
-      <c r="EA151" s="165">
+      <c r="EA151" s="163">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="EB151" s="165">
+      <c r="EB151" s="163">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -57443,11 +57450,11 @@
       <c r="DY152" s="29" t="s">
         <v>1727</v>
       </c>
-      <c r="EA152" s="165">
+      <c r="EA152" s="163">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="EB152" s="165">
+      <c r="EB152" s="163">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -58005,11 +58012,11 @@
       <c r="DY154" s="29" t="s">
         <v>491</v>
       </c>
-      <c r="EA154" s="165">
+      <c r="EA154" s="163">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="EB154" s="165">
+      <c r="EB154" s="163">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -58376,11 +58383,11 @@
       <c r="DY155" s="29" t="s">
         <v>2696</v>
       </c>
-      <c r="EA155" s="165">
+      <c r="EA155" s="163">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="EB155" s="165">
+      <c r="EB155" s="163">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -58743,7 +58750,7 @@
         <v>0.77753399199999995</v>
       </c>
       <c r="DU156" s="90"/>
-      <c r="DV156" s="169">
+      <c r="DV156" s="167">
         <v>-3.4000000000000002E-2</v>
       </c>
       <c r="DW156" s="148"/>
@@ -58753,11 +58760,11 @@
       <c r="DY156" s="29" t="s">
         <v>1013</v>
       </c>
-      <c r="EA156" s="165">
+      <c r="EA156" s="163">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="EB156" s="165">
+      <c r="EB156" s="163">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -59496,11 +59503,11 @@
       <c r="DY159" s="29" t="s">
         <v>291</v>
       </c>
-      <c r="EA159" s="165">
+      <c r="EA159" s="163">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="EB159" s="165">
+      <c r="EB159" s="163">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
@@ -59934,11 +59941,11 @@
       <c r="CO161" s="37" t="s">
         <v>274</v>
       </c>
-      <c r="CP161" s="151" t="s">
+      <c r="CP161" s="172" t="s">
         <v>2764</v>
       </c>
-      <c r="CQ161" s="152"/>
-      <c r="CR161" s="152"/>
+      <c r="CQ161" s="173"/>
+      <c r="CR161" s="173"/>
       <c r="CS161" s="37" t="s">
         <v>278</v>
       </c>
@@ -60380,11 +60387,11 @@
       <c r="DY162" s="29" t="s">
         <v>2784</v>
       </c>
-      <c r="EA162" s="165">
+      <c r="EA162" s="163">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="EB162" s="165">
+      <c r="EB162" s="163">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -60991,11 +60998,11 @@
       <c r="CO165" s="37" t="s">
         <v>330</v>
       </c>
-      <c r="CP165" s="151" t="s">
+      <c r="CP165" s="172" t="s">
         <v>2815</v>
       </c>
-      <c r="CQ165" s="152"/>
-      <c r="CR165" s="152"/>
+      <c r="CQ165" s="173"/>
+      <c r="CR165" s="173"/>
       <c r="CS165" s="37" t="s">
         <v>681</v>
       </c>
@@ -61421,7 +61428,7 @@
         <v>0.210207014</v>
       </c>
       <c r="DU166" s="90"/>
-      <c r="DV166" s="153">
+      <c r="DV166" s="151">
         <f>-0.175454592</f>
         <v>-0.17545459199999999</v>
       </c>
@@ -61432,11 +61439,11 @@
       <c r="DY166" s="29" t="s">
         <v>2838</v>
       </c>
-      <c r="EA166" s="165">
+      <c r="EA166" s="163">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="EB166" s="165">
+      <c r="EB166" s="163">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -61986,11 +61993,11 @@
       <c r="DY168" s="29" t="s">
         <v>2862</v>
       </c>
-      <c r="EA168" s="165">
+      <c r="EA168" s="163">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="EB168" s="165">
+      <c r="EB168" s="163">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -62212,11 +62219,11 @@
       <c r="DS170" s="90"/>
       <c r="DT170" s="147"/>
       <c r="DU170" s="45"/>
-      <c r="DV170" s="165"/>
+      <c r="DV170" s="163"/>
       <c r="DW170" s="90"/>
       <c r="DX170" s="45"/>
       <c r="DY170" s="45"/>
-      <c r="EC170" s="165"/>
+      <c r="EC170" s="163"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>